<commit_message>
Added tests (and new data) for ensuring that the title is
correct, and that danish special chars and whitespace do not make it into
permission values.
</commit_message>
<xml_diff>
--- a/AutomationTest/Bruger rettigheder 07022014.xlsx
+++ b/AutomationTest/Bruger rettigheder 07022014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="1440" windowWidth="36620" windowHeight="22220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30420" windowHeight="18920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
@@ -434,16 +434,16 @@
     <t>SoegeEfterTidligereJournalerForAktuellePatient</t>
   </si>
   <si>
-    <t>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/mobil</t>
-  </si>
-  <si>
-    <t>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/central</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t xml:space="preserve">x </t>
+  </si>
+  <si>
+    <t>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj/mobil</t>
+  </si>
+  <si>
+    <t>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj/central</t>
   </si>
 </sst>
 </file>
@@ -1265,6 +1265,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1282,12 +1288,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1588,7 +1588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1661,13 +1661,14 @@
   </sheetPr>
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="4.33203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="60" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.83203125" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91" style="143" customWidth="1"/>
     <col min="4" max="4" width="86.5" style="92" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" style="92" customWidth="1"/>
@@ -1683,10 +1684,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="39" customHeight="1">
-      <c r="C1" s="144" t="s">
+      <c r="C1" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="144"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="101"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
@@ -1703,20 +1704,20 @@
       <c r="C2" s="130"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="145" t="s">
+      <c r="F2" s="147" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="148" t="s">
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="150" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="151"/>
+      <c r="O2" s="151"/>
       <c r="P2" s="102"/>
     </row>
     <row r="3" spans="1:16" s="33" customFormat="1" ht="76.5" customHeight="1">
@@ -1803,9 +1804,9 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="150" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="144" t="s">
         <v>123</v>
       </c>
       <c r="C6" s="134" t="s">
@@ -1873,9 +1874,9 @@
     </row>
     <row r="9" spans="1:16" ht="30">
       <c r="A9" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="145" t="s">
         <v>124</v>
       </c>
       <c r="C9" s="134" t="s">
@@ -1903,7 +1904,7 @@
     </row>
     <row r="10" spans="1:16" ht="30">
       <c r="A10" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B10" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C10,"æ","ae"),"ø","oe"),"å","aa"),"Æ","Ae"),"Ø","Oe"),"Å","Aa")," ","")</f>
@@ -1934,7 +1935,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B11" s="10" t="str">
         <f t="shared" ref="B11:B74" si="0">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C11,"æ","ae"),"ø","oe"),"å","aa"),"Æ","Ae"),"Ø","Oe"),"Å","Aa")," ","")</f>
@@ -2007,7 +2008,7 @@
     </row>
     <row r="14" spans="1:16" ht="30">
       <c r="A14" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B14" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2040,7 +2041,7 @@
     </row>
     <row r="15" spans="1:16" ht="30">
       <c r="A15" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B15" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2071,7 +2072,7 @@
     </row>
     <row r="16" spans="1:16" s="118" customFormat="1">
       <c r="A16" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B16" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2146,7 +2147,7 @@
     </row>
     <row r="19" spans="1:16" ht="23.25" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B19" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2177,7 +2178,7 @@
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B20" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2208,7 +2209,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B21" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2239,7 +2240,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B22" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2272,7 +2273,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B23" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2347,7 +2348,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B26" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2378,7 +2379,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B27" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2409,7 +2410,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B28" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2481,7 +2482,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B31" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2583,7 +2584,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B36" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2613,7 +2614,7 @@
     </row>
     <row r="37" spans="1:16" s="118" customFormat="1">
       <c r="A37" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B37" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2685,7 +2686,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B40" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2717,7 +2718,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B41" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2747,7 +2748,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B42" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2799,7 +2800,7 @@
     </row>
     <row r="44" spans="1:16" ht="30">
       <c r="A44" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B44" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2829,7 +2830,7 @@
     </row>
     <row r="45" spans="1:16" s="118" customFormat="1" ht="30">
       <c r="A45" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B45" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2942,7 +2943,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B50" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2976,7 +2977,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B51" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3008,7 +3009,7 @@
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B52" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3060,7 +3061,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B54" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3092,7 +3093,7 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B55" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3124,7 +3125,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B56" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3195,7 +3196,7 @@
     </row>
     <row r="59" spans="1:16" ht="30">
       <c r="A59" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B59" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3227,7 +3228,7 @@
     </row>
     <row r="60" spans="1:16" ht="30">
       <c r="A60" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B60" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3298,7 +3299,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B63" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3323,14 +3324,14 @@
       <c r="K63" s="76"/>
       <c r="L63" s="77"/>
       <c r="M63" s="77" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N63" s="77"/>
       <c r="O63" s="78"/>
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B64" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3354,7 +3355,7 @@
       <c r="I64" s="81"/>
       <c r="J64" s="82"/>
       <c r="K64" s="83" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L64" s="84"/>
       <c r="M64" s="84"/>
@@ -3363,7 +3364,7 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B65" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3393,7 +3394,7 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B66" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3418,14 +3419,14 @@
       <c r="K66" s="83"/>
       <c r="L66" s="84"/>
       <c r="M66" s="84" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N66" s="84"/>
       <c r="O66" s="85"/>
     </row>
     <row r="67" spans="1:16">
       <c r="A67" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B67" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3496,7 +3497,7 @@
     </row>
     <row r="70" spans="1:16" s="118" customFormat="1">
       <c r="A70" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B70" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3527,7 +3528,7 @@
     </row>
     <row r="71" spans="1:16" s="118" customFormat="1" ht="34.5" customHeight="1">
       <c r="A71" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B71" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3558,7 +3559,7 @@
     </row>
     <row r="72" spans="1:16" s="118" customFormat="1">
       <c r="A72" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B72" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3589,7 +3590,7 @@
     </row>
     <row r="73" spans="1:16" s="118" customFormat="1" ht="34.5" customHeight="1">
       <c r="A73" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B73" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3661,7 +3662,7 @@
     </row>
     <row r="76" spans="1:16" s="118" customFormat="1">
       <c r="A76" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B76" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3692,7 +3693,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B77" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3722,7 +3723,7 @@
     </row>
     <row r="78" spans="1:16" ht="30">
       <c r="A78" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B78" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3780,7 +3781,7 @@
     </row>
     <row r="81" spans="1:15" ht="52.5" customHeight="1">
       <c r="A81" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B81" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3812,7 +3813,7 @@
     </row>
     <row r="82" spans="1:15" ht="30">
       <c r="A82" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B82" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3844,7 +3845,7 @@
     </row>
     <row r="83" spans="1:15" ht="30">
       <c r="A83" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B83" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3876,7 +3877,7 @@
     </row>
     <row r="84" spans="1:15" ht="20.25" customHeight="1">
       <c r="A84" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B84" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3908,7 +3909,7 @@
     </row>
     <row r="85" spans="1:15" ht="21" customHeight="1">
       <c r="A85" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B85" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3940,7 +3941,7 @@
     </row>
     <row r="86" spans="1:15" ht="23.25" customHeight="1">
       <c r="A86" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B86" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3972,7 +3973,7 @@
     </row>
     <row r="87" spans="1:15">
       <c r="A87" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B87" s="10" t="str">
         <f t="shared" si="1"/>
@@ -4002,7 +4003,7 @@
     </row>
     <row r="88" spans="1:15">
       <c r="A88" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B88" s="10" t="str">
         <f t="shared" si="1"/>
@@ -4032,7 +4033,7 @@
     </row>
     <row r="89" spans="1:15">
       <c r="A89" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B89" s="10" t="str">
         <f t="shared" si="1"/>
@@ -4057,7 +4058,7 @@
       <c r="K89" s="28"/>
       <c r="L89" s="28"/>
       <c r="M89" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N89" s="28"/>
       <c r="O89" s="29"/>

</xml_diff>